<commit_message>
Added query to reset counter to 1 in ACCESS db
</commit_message>
<xml_diff>
--- a/Tickets.xlsx
+++ b/Tickets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GinaG\Documents\Cravings-Restaurant-Reservation-System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GinaG\Documents\CRRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="161">
   <si>
     <t>Tickets</t>
   </si>
@@ -443,15 +443,9 @@
     <t>Day(s)</t>
   </si>
   <si>
-    <t>3/21-3/27</t>
-  </si>
-  <si>
     <t>2/26-3/17</t>
   </si>
   <si>
-    <t>3/20-3/27</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -476,9 +470,6 @@
     <t>Domi, Gina</t>
   </si>
   <si>
-    <t>3/25-3/27</t>
-  </si>
-  <si>
     <t>12 hrs</t>
   </si>
   <si>
@@ -495,6 +486,24 @@
   </si>
   <si>
     <t>Mara, Joyce</t>
+  </si>
+  <si>
+    <t>15 mins</t>
+  </si>
+  <si>
+    <t>3/20-3/30</t>
+  </si>
+  <si>
+    <t>3/25-3/30</t>
+  </si>
+  <si>
+    <t>3/21-3/30</t>
+  </si>
+  <si>
+    <t>2/10-03/30</t>
+  </si>
+  <si>
+    <t>Gina, Domi</t>
   </si>
 </sst>
 </file>
@@ -602,19 +611,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -921,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,12 +945,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -964,12 +973,12 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
       <c r="F3" s="4" t="s">
         <v>90</v>
       </c>
@@ -1100,7 +1109,7 @@
         <v>137</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>55</v>
@@ -1110,12 +1119,12 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1164,7 +1173,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>114</v>
@@ -1178,7 +1187,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>114</v>
@@ -1188,12 +1197,12 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1850,20 +1859,20 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+      <c r="A71" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B71" s="15"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
@@ -1873,7 +1882,7 @@
         <v>43178</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>100</v>
@@ -1887,7 +1896,7 @@
         <v>43178</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>100</v>
@@ -1895,13 +1904,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B75" s="7">
         <v>43178</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>7</v>
@@ -1909,7 +1918,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B76" s="7">
         <v>43178</v>
@@ -1925,9 +1934,9 @@
       <c r="A77" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
@@ -1954,7 +1963,7 @@
         <v>96</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1979,10 +1988,10 @@
         <v>43178</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1990,22 +1999,22 @@
         <v>107</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>114</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>56</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B83" s="17"/>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
@@ -2040,7 +2049,7 @@
         <v>110</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>114</v>
@@ -2053,16 +2062,16 @@
       <c r="A87" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B87" s="17"/>
-      <c r="C87" s="17"/>
-      <c r="D87" s="17"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>114</v>
@@ -2076,13 +2085,13 @@
         <v>112</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>114</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>56</v>
+        <v>160</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2090,7 +2099,7 @@
         <v>113</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>114</v>
@@ -2100,19 +2109,19 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="15" t="s">
+      <c r="A91" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B91" s="15"/>
-      <c r="C91" s="15"/>
-      <c r="D91" s="15"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="17"/>
+      <c r="D91" s="17"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>114</v>
@@ -2126,13 +2135,13 @@
         <v>30</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>114</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2140,13 +2149,13 @@
         <v>31</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>114</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2154,29 +2163,29 @@
         <v>32</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>114</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="15" t="s">
+      <c r="A96" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B96" s="15"/>
-      <c r="C96" s="15"/>
-      <c r="D96" s="15"/>
+      <c r="B96" s="17"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="17"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>114</v>
@@ -2190,7 +2199,7 @@
         <v>35</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>114</v>
@@ -2204,7 +2213,7 @@
         <v>36</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>114</v>
@@ -2218,7 +2227,7 @@
         <v>37</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>114</v>
@@ -2232,7 +2241,7 @@
         <v>38</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>114</v>
@@ -2242,12 +2251,12 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="15" t="s">
+      <c r="A102" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B102" s="15"/>
-      <c r="C102" s="15"/>
-      <c r="D102" s="15"/>
+      <c r="B102" s="17"/>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
@@ -2274,7 +2283,7 @@
         <v>52</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2282,10 +2291,10 @@
         <v>42</v>
       </c>
       <c r="B105" s="7">
-        <v>43186</v>
+        <v>43189</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>87</v>
@@ -2296,52 +2305,52 @@
         <v>43</v>
       </c>
       <c r="B106" s="12">
-        <v>43186</v>
+        <v>43189</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="18" t="s">
-        <v>155</v>
+      <c r="A107" s="15" t="s">
+        <v>152</v>
       </c>
       <c r="B107" s="7">
         <v>43186</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="18" t="s">
-        <v>153</v>
+      <c r="A108" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="B108" s="7">
-        <v>43186</v>
+        <v>43189</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>96</v>
+        <v>155</v>
       </c>
       <c r="D108" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="18" t="s">
-        <v>154</v>
+      <c r="A109" s="15" t="s">
+        <v>151</v>
       </c>
       <c r="B109" s="7">
-        <v>43186</v>
+        <v>43189</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>96</v>
+        <v>155</v>
       </c>
       <c r="D109" s="8" t="s">
         <v>8</v>
@@ -2349,11 +2358,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="A91:D91"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A96:D96"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
@@ -2367,6 +2371,11 @@
     <mergeCell ref="B50:D50"/>
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A96:D96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>